<commit_message>
dsada Co-authored-by: SkjalgN <SkjalgN@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Task4/Villa.xlsx
+++ b/Task4/Villa.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antoira\Documents\Work\Enseignement\NTNU\NTNU - TPK4186 - Advanced Tools for Performance Engineering\Assignments\2023\Construction Project\Program\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christian/performanceengineering/Task4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB3555C-128A-47F0-9F49-1D1FDD8FD175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B258D2DD-4FC4-7C4F-A253-FB27C400EFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23140" yWindow="1980" windowWidth="38640" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Villa" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -826,19 +839,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I69" sqref="I69"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -855,7 +868,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>143</v>
       </c>
@@ -866,14 +879,14 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -890,7 +903,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -907,7 +920,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -924,7 +937,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -941,7 +954,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -958,7 +971,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -975,7 +988,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -992,7 +1005,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1009,7 +1022,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1026,7 +1039,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1043,7 +1056,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1060,7 +1073,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1077,7 +1090,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1094,7 +1107,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1111,7 +1124,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -1128,7 +1141,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1145,7 +1158,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -1162,7 +1175,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -1179,7 +1192,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1196,7 +1209,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -1213,7 +1226,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -1230,7 +1243,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -1247,7 +1260,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -1264,7 +1277,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -1281,7 +1294,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -1298,7 +1311,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -1315,7 +1328,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -1332,7 +1345,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -1349,7 +1362,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -1366,7 +1379,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -1383,7 +1396,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -1400,7 +1413,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -1417,7 +1430,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -1434,24 +1447,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>5</v>
-      </c>
-      <c r="B46" t="s">
-        <v>80</v>
-      </c>
-      <c r="C46" t="s">
-        <v>81</v>
-      </c>
-      <c r="D46" t="s">
-        <v>43</v>
-      </c>
-      <c r="E46" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -1468,7 +1464,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>5</v>
       </c>
@@ -1485,7 +1481,24 @@
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" t="s">
+        <v>43</v>
+      </c>
+      <c r="E49" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -1502,7 +1515,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -1519,7 +1532,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>5</v>
       </c>
@@ -1536,7 +1549,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>5</v>
       </c>
@@ -1553,7 +1566,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>5</v>
       </c>
@@ -1570,7 +1583,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>5</v>
       </c>
@@ -1587,7 +1600,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>5</v>
       </c>
@@ -1604,7 +1617,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>5</v>
       </c>
@@ -1621,7 +1634,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>5</v>
       </c>
@@ -1638,7 +1651,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>5</v>
       </c>
@@ -1655,7 +1668,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>5</v>
       </c>
@@ -1672,7 +1685,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>5</v>
       </c>
@@ -1689,7 +1702,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>5</v>
       </c>
@@ -1706,7 +1719,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>5</v>
       </c>
@@ -1723,7 +1736,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>5</v>
       </c>
@@ -1740,7 +1753,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>5</v>
       </c>
@@ -1757,7 +1770,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>5</v>
       </c>
@@ -1774,7 +1787,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>5</v>
       </c>
@@ -1791,7 +1804,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>5</v>
       </c>
@@ -1808,7 +1821,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>5</v>
       </c>
@@ -1825,7 +1838,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>5</v>
       </c>
@@ -1842,7 +1855,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>5</v>
       </c>
@@ -1859,7 +1872,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>5</v>
       </c>
@@ -1876,7 +1889,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>5</v>
       </c>
@@ -1893,7 +1906,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>5</v>
       </c>
@@ -1910,7 +1923,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>143</v>
       </c>

</xml_diff>